<commit_message>
Settings Sheet added to .xlsx
</commit_message>
<xml_diff>
--- a/data/leaguedatatest.xlsx
+++ b/data/leaguedatatest.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Settings" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="37">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -149,6 +150,15 @@
   </si>
   <si>
     <t xml:space="preserve">19/04/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">League Champions Pot</t>
   </si>
 </sst>
 </file>
@@ -264,7 +274,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -298,6 +308,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -552,7 +566,7 @@
   </sheetPr>
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E43" activeCellId="0" sqref="E43"/>
     </sheetView>
   </sheetViews>
@@ -1492,4 +1506,44 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="9" t="n">
+        <v>188.69</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>